<commit_message>
Add the first runs with a full dataset
</commit_message>
<xml_diff>
--- a/Bulk_Processing_Log.xlsx
+++ b/Bulk_Processing_Log.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16200" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Runs" sheetId="1" r:id="rId1"/>
+    <sheet name="Disk usage" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,8 +28,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>James Dempsey</author>
+  </authors>
+  <commentList>
+    <comment ref="F4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>James Dempsey:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Analyse failed as  bane not on path. Reran analyse steps</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t>Stats</t>
   </si>
@@ -48,9 +81,6 @@
     <t>Spectra produced</t>
   </si>
   <si>
-    <t>Decent S/N</t>
-  </si>
-  <si>
     <t>Settings</t>
   </si>
   <si>
@@ -120,14 +150,66 @@
     <t>Rerun plot-ly only</t>
   </si>
   <si>
-    <t>Full reprocess</t>
+    <t>Full reprocess, added 0km/s flagging</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Gaskap</t>
+  </si>
+  <si>
+    <t>Add interval to cal, add some flagging</t>
+  </si>
+  <si>
+    <t>No interval on phase cal, extra flagging, extra days</t>
+  </si>
+  <si>
+    <t>% cubes</t>
+  </si>
+  <si>
+    <t>% good fields</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Fields</t>
+  </si>
+  <si>
+    <t>Cubes</t>
+  </si>
+  <si>
+    <t>6a</t>
+  </si>
+  <si>
+    <t>6b</t>
+  </si>
+  <si>
+    <t>6c</t>
+  </si>
+  <si>
+    <t>Spectra w/decent S/N</t>
+  </si>
+  <si>
+    <t>% good spectra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -156,6 +238,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -194,28 +287,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -489,23 +600,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
@@ -516,52 +630,98 @@
       <c r="D1">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="B2" s="10">
+        <v>42620</v>
+      </c>
       <c r="C2" s="2">
         <v>42623</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>42634</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>42634</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="3">
+        <v>42638</v>
+      </c>
+      <c r="G2" s="3">
+        <v>42642</v>
+      </c>
+      <c r="H2" s="3">
+        <v>42644</v>
+      </c>
+      <c r="I2" s="3">
+        <v>42644</v>
+      </c>
+      <c r="J2" s="3">
+        <v>42645</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.95208333333333339</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.95208333333333339</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.68333333333333324</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.33263888888888887</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="D3" s="5">
-        <v>0.95208333333333339</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0.95208333333333339</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1"/>
+      <c r="D4" s="4">
+        <v>0.3972222222222222</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.3972222222222222</v>
+      </c>
+      <c r="F4" s="4">
+        <v>6.8749999999999992E-2</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.12847222222222224</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="D4" s="5">
-        <v>0.3972222222222222</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0.3972222222222222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="B5" s="1"/>
       <c r="D5">
@@ -570,31 +730,53 @@
       <c r="E5">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>11</v>
+      </c>
+      <c r="F7">
+        <v>11</v>
+      </c>
+      <c r="G7">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>11</v>
+      </c>
+      <c r="I7">
+        <v>11</v>
+      </c>
+      <c r="J7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7">
-        <v>11</v>
-      </c>
-      <c r="D7">
-        <v>11</v>
-      </c>
-      <c r="E7">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="1"/>
+      <c r="B8">
+        <v>21</v>
+      </c>
       <c r="C8">
         <v>21</v>
       </c>
@@ -604,12 +786,30 @@
       <c r="E8">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>21</v>
+      </c>
+      <c r="G8" s="9">
+        <v>26</v>
+      </c>
+      <c r="H8" s="9">
+        <v>43</v>
+      </c>
+      <c r="I8" s="9">
+        <v>43</v>
+      </c>
+      <c r="J8" s="9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <f>B8-B7+1</f>
+        <v>11</v>
+      </c>
       <c r="C9">
         <f>C8-C7+1</f>
         <v>11</v>
@@ -620,22 +820,38 @@
       <c r="E9">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>11</v>
+      </c>
+      <c r="G9">
+        <f>G8-G7+1</f>
+        <v>16</v>
+      </c>
+      <c r="H9">
+        <v>33</v>
+      </c>
+      <c r="I9">
+        <v>33</v>
+      </c>
+      <c r="J9">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12">
+        <v>11</v>
+      </c>
       <c r="C12">
         <v>11</v>
       </c>
@@ -645,12 +861,29 @@
       <c r="E12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <v>11</v>
+      </c>
+      <c r="G12">
+        <v>16</v>
+      </c>
+      <c r="H12">
+        <v>33</v>
+      </c>
+      <c r="I12">
+        <v>33</v>
+      </c>
+      <c r="J12" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13">
+        <v>198</v>
+      </c>
       <c r="C13">
         <v>198</v>
       </c>
@@ -660,8 +893,23 @@
       <c r="E13">
         <v>198</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <v>198</v>
+      </c>
+      <c r="G13">
+        <v>292</v>
+      </c>
+      <c r="H13">
+        <v>368</v>
+      </c>
+      <c r="I13">
+        <v>368</v>
+      </c>
+      <c r="J13" s="6">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -669,20 +917,29 @@
       <c r="C14">
         <v>100</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="6">
         <v>107</v>
       </c>
       <c r="E14">
         <v>107</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="6">
+        <v>109</v>
+      </c>
+      <c r="G14">
+        <v>151</v>
+      </c>
+      <c r="J14">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -690,196 +947,753 @@
       <c r="C16">
         <v>549</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="6">
         <v>427</v>
       </c>
       <c r="E16">
         <v>427</v>
       </c>
+      <c r="F16" s="6">
+        <v>399</v>
+      </c>
+      <c r="G16">
+        <v>543</v>
+      </c>
+      <c r="H16" s="6">
+        <v>631</v>
+      </c>
+      <c r="I16">
+        <v>631</v>
+      </c>
+      <c r="J16" s="6">
+        <v>1019</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17">
         <v>110</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="6">
         <v>113</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>72</v>
+      </c>
+      <c r="F17" s="6">
+        <v>81</v>
+      </c>
+      <c r="G17" s="6">
+        <v>94</v>
+      </c>
+      <c r="H17" s="6">
+        <v>156</v>
+      </c>
+      <c r="I17" s="6">
+        <v>117</v>
+      </c>
+      <c r="J17" s="6">
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1"/>
       <c r="D18">
         <v>91</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>38</v>
       </c>
+      <c r="F18" s="6">
+        <v>41</v>
+      </c>
+      <c r="G18">
+        <v>56</v>
+      </c>
+      <c r="H18">
+        <v>84</v>
+      </c>
+      <c r="I18">
+        <v>71</v>
+      </c>
+      <c r="J18" s="6">
+        <v>110</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="16">
+        <f>B14/B13</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="16">
+        <f t="shared" ref="C19:G19" si="0">C14/C13</f>
+        <v>0.50505050505050508</v>
+      </c>
+      <c r="D19" s="16">
+        <f t="shared" si="0"/>
+        <v>0.54040404040404044</v>
+      </c>
+      <c r="E19" s="16">
+        <f t="shared" si="0"/>
+        <v>0.54040404040404044</v>
+      </c>
+      <c r="F19" s="16">
+        <f t="shared" si="0"/>
+        <v>0.5505050505050505</v>
+      </c>
+      <c r="G19" s="16">
+        <f t="shared" si="0"/>
+        <v>0.51712328767123283</v>
+      </c>
+      <c r="H19" s="16">
+        <f t="shared" ref="H19:I19" si="1">H14/H13</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="16">
+        <f t="shared" ref="J19" si="2">J14/J13</f>
+        <v>0.50929368029739774</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="B20" s="16">
+        <f>B18/B13</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="16">
+        <f t="shared" ref="C20:G20" si="3">C18/C13</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="16">
+        <f t="shared" si="3"/>
+        <v>0.45959595959595961</v>
+      </c>
+      <c r="E20" s="16">
+        <f t="shared" si="3"/>
+        <v>0.19191919191919191</v>
+      </c>
+      <c r="F20" s="16">
+        <f t="shared" si="3"/>
+        <v>0.20707070707070707</v>
+      </c>
+      <c r="G20" s="16">
+        <f t="shared" si="3"/>
+        <v>0.19178082191780821</v>
+      </c>
+      <c r="H20" s="16">
+        <f t="shared" ref="H20:I20" si="4">H18/H13</f>
+        <v>0.22826086956521738</v>
+      </c>
+      <c r="I20" s="16">
+        <f t="shared" si="4"/>
+        <v>0.19293478260869565</v>
+      </c>
+      <c r="J20" s="16">
+        <f t="shared" ref="J20" si="5">J18/J13</f>
+        <v>0.20446096654275092</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="C21">
-        <v>-15</v>
-      </c>
-      <c r="D21">
-        <v>-15</v>
-      </c>
-      <c r="E21" s="6">
-        <v>-8</v>
+        <v>44</v>
+      </c>
+      <c r="B21" s="16">
+        <f>IF(B16=0,0,B17/B16)</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="16">
+        <f t="shared" ref="C21:J21" si="6">IF(C16=0,0,C17/C16)</f>
+        <v>0.20036429872495445</v>
+      </c>
+      <c r="D21" s="16">
+        <f t="shared" si="6"/>
+        <v>0.26463700234192039</v>
+      </c>
+      <c r="E21" s="16">
+        <f t="shared" si="6"/>
+        <v>0.16861826697892271</v>
+      </c>
+      <c r="F21" s="16">
+        <f t="shared" si="6"/>
+        <v>0.20300751879699247</v>
+      </c>
+      <c r="G21" s="16">
+        <f t="shared" si="6"/>
+        <v>0.17311233885819521</v>
+      </c>
+      <c r="H21" s="16">
+        <f t="shared" si="6"/>
+        <v>0.24722662440570523</v>
+      </c>
+      <c r="I21" s="16">
+        <f t="shared" si="6"/>
+        <v>0.18541996830427893</v>
+      </c>
+      <c r="J21" s="16">
+        <f t="shared" si="6"/>
+        <v>0.2139352306182532</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B22" s="1"/>
-      <c r="C22">
-        <v>10</v>
-      </c>
-      <c r="D22">
-        <v>10</v>
-      </c>
-      <c r="E22" s="6">
-        <v>6</v>
-      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="C23">
-        <v>10</v>
+        <v>-15</v>
       </c>
       <c r="D23">
-        <v>10</v>
-      </c>
-      <c r="E23">
-        <v>10</v>
+        <v>-15</v>
+      </c>
+      <c r="E23" s="5">
+        <v>-8</v>
+      </c>
+      <c r="F23">
+        <v>-8</v>
+      </c>
+      <c r="G23">
+        <v>-8</v>
+      </c>
+      <c r="H23">
+        <v>-8</v>
+      </c>
+      <c r="I23" s="5">
+        <v>-4</v>
+      </c>
+      <c r="J23">
+        <v>-4</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="C24">
-        <v>0.02</v>
+        <v>10</v>
       </c>
       <c r="D24">
-        <v>0.02</v>
-      </c>
-      <c r="E24">
-        <v>0.02</v>
+        <v>10</v>
+      </c>
+      <c r="E24" s="5">
+        <v>6</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>6</v>
+      </c>
+      <c r="H24">
+        <v>6</v>
+      </c>
+      <c r="I24" s="5">
+        <v>4</v>
+      </c>
+      <c r="J24">
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="13">
         <v>10</v>
       </c>
-      <c r="B25" s="1"/>
       <c r="C25">
-        <v>1.3</v>
+        <v>10</v>
       </c>
       <c r="D25">
-        <v>1.3</v>
+        <v>10</v>
       </c>
       <c r="E25">
-        <v>1.3</v>
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <v>10</v>
+      </c>
+      <c r="G25">
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <v>10</v>
+      </c>
+      <c r="I25">
+        <v>10</v>
+      </c>
+      <c r="J25">
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="C26">
-        <v>0.8</v>
-      </c>
-      <c r="D26">
-        <v>0.8</v>
+        <v>0.01</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0.02</v>
       </c>
       <c r="E26">
-        <v>0.8</v>
+        <v>0.02</v>
+      </c>
+      <c r="F26">
+        <v>0.02</v>
+      </c>
+      <c r="G26">
+        <v>0.02</v>
+      </c>
+      <c r="H26">
+        <v>0.02</v>
+      </c>
+      <c r="I26">
+        <v>0.02</v>
+      </c>
+      <c r="J26">
+        <v>0.02</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27">
+        <v>1.3</v>
+      </c>
+      <c r="D27">
+        <v>1.3</v>
+      </c>
+      <c r="E27">
+        <v>1.3</v>
+      </c>
+      <c r="F27">
+        <v>1.3</v>
+      </c>
+      <c r="G27">
+        <v>1.3</v>
+      </c>
+      <c r="H27">
+        <v>1.3</v>
+      </c>
+      <c r="I27">
+        <v>1.3</v>
+      </c>
+      <c r="J27">
+        <v>1.3</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="C28">
+        <v>0.8</v>
+      </c>
+      <c r="D28">
+        <v>0.8</v>
+      </c>
+      <c r="E28">
+        <v>0.8</v>
+      </c>
+      <c r="F28">
+        <v>0.8</v>
+      </c>
+      <c r="G28">
+        <v>0.8</v>
+      </c>
+      <c r="H28">
+        <v>0.8</v>
+      </c>
+      <c r="I28">
+        <v>0.8</v>
+      </c>
+      <c r="J28">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D28" t="s">
-        <v>24</v>
-      </c>
-      <c r="E28" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="B30" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" t="s">
+        <v>23</v>
+      </c>
+      <c r="I30" t="s">
+        <v>23</v>
+      </c>
+      <c r="J30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
+      <c r="F32" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="15">
+        <v>42638</v>
+      </c>
+      <c r="B2">
+        <v>835</v>
+      </c>
+      <c r="C2">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="15">
+        <v>42642</v>
+      </c>
+      <c r="B3">
+        <v>1400</v>
+      </c>
+      <c r="C3">
+        <v>4100</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <f>SUM(B2:B17)</f>
+        <v>292</v>
+      </c>
+      <c r="C19">
+        <f>SUM(C2:C17)</f>
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add a new longitude-velocity plot which includes a profile of HI emission from the GASS III dataset.
</commit_message>
<xml_diff>
--- a/Bulk_Processing_Log.xlsx
+++ b/Bulk_Processing_Log.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16200" tabRatio="500"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Runs" sheetId="1" r:id="rId1"/>
@@ -56,12 +56,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="K9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>James Dempsey:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Skipping day 24 which has bad bp cal</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
   <si>
     <t>Stats</t>
   </si>
@@ -196,6 +218,15 @@
   </si>
   <si>
     <t>% good spectra</t>
+  </si>
+  <si>
+    <t>Excluded day 24 from all processing</t>
+  </si>
+  <si>
+    <t>Processing errors</t>
+  </si>
+  <si>
+    <t>Clean niter=250</t>
   </si>
 </sst>
 </file>
@@ -293,7 +324,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -321,6 +352,8 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -601,13 +634,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomRight" activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,9 +648,11 @@
     <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -648,8 +683,14 @@
       <c r="J1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1">
+        <v>7</v>
+      </c>
+      <c r="L1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -680,8 +721,14 @@
       <c r="J2" s="3">
         <v>42645</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="3">
+        <v>42661</v>
+      </c>
+      <c r="L2" s="3">
+        <v>42668</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -700,8 +747,14 @@
       <c r="G3" s="4">
         <v>0.33263888888888887</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" s="4">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0.88124999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -718,8 +771,14 @@
       <c r="G4" s="4">
         <v>0.12847222222222224</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" s="17">
+        <v>42664.024305555555</v>
+      </c>
+      <c r="L4" s="17">
+        <v>42669.988888888889</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -733,12 +792,18 @@
       <c r="G5">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" s="18">
+        <v>2.1076388888888888</v>
+      </c>
+      <c r="L5" s="18">
+        <v>1.1076388888888888</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -769,8 +834,14 @@
       <c r="J7">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <v>11</v>
+      </c>
+      <c r="L7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -801,8 +872,14 @@
       <c r="J8" s="9">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" s="9">
+        <v>43</v>
+      </c>
+      <c r="L8" s="9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -836,16 +913,22 @@
       <c r="J9">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" s="5">
+        <v>32</v>
+      </c>
+      <c r="L9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -876,8 +959,17 @@
       <c r="J12" s="5">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12">
+        <v>32</v>
+      </c>
+      <c r="L12">
+        <v>32</v>
+      </c>
+      <c r="M12">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -908,8 +1000,17 @@
       <c r="J13" s="6">
         <v>538</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13" s="6">
+        <v>522</v>
+      </c>
+      <c r="L13">
+        <v>522</v>
+      </c>
+      <c r="M13">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -932,299 +1033,372 @@
       <c r="J14">
         <v>274</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14" s="6">
+        <v>310</v>
+      </c>
+      <c r="L14">
+        <v>310</v>
+      </c>
+      <c r="M14">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="F15">
+        <v>13</v>
+      </c>
+      <c r="G15">
+        <v>15</v>
+      </c>
+      <c r="J15">
+        <v>23</v>
+      </c>
+      <c r="K15">
+        <v>18</v>
+      </c>
+      <c r="L15">
+        <v>18</v>
+      </c>
+      <c r="M15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16">
-        <v>549</v>
-      </c>
-      <c r="D16" s="6">
-        <v>427</v>
-      </c>
-      <c r="E16">
-        <v>427</v>
-      </c>
-      <c r="F16" s="6">
-        <v>399</v>
-      </c>
-      <c r="G16">
-        <v>543</v>
-      </c>
-      <c r="H16" s="6">
-        <v>631</v>
-      </c>
-      <c r="I16">
-        <v>631</v>
-      </c>
-      <c r="J16" s="6">
-        <v>1019</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17">
+        <v>549</v>
+      </c>
+      <c r="D17" s="6">
+        <v>427</v>
+      </c>
+      <c r="E17">
+        <v>427</v>
+      </c>
+      <c r="F17" s="6">
+        <v>399</v>
+      </c>
+      <c r="G17">
+        <v>543</v>
+      </c>
+      <c r="H17" s="6">
+        <v>631</v>
+      </c>
+      <c r="I17">
+        <v>631</v>
+      </c>
+      <c r="J17" s="6">
+        <v>1019</v>
+      </c>
+      <c r="K17" s="6">
+        <v>999</v>
+      </c>
+      <c r="L17" s="6">
+        <v>1310</v>
+      </c>
+      <c r="M17">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18">
         <v>110</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D18" s="6">
         <v>113</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E18" s="6">
         <v>72</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F18" s="6">
         <v>81</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G18" s="6">
         <v>94</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H18" s="6">
         <v>156</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I18" s="6">
         <v>117</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J18" s="6">
         <v>218</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="K18" s="6">
+        <v>220</v>
+      </c>
+      <c r="L18" s="6">
+        <v>609</v>
+      </c>
+      <c r="M18" s="6">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="D18">
+      <c r="B19" s="1"/>
+      <c r="D19">
         <v>91</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E19" s="6">
         <v>38</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F19" s="6">
         <v>41</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <v>56</v>
       </c>
-      <c r="H18">
+      <c r="H19">
         <v>84</v>
       </c>
-      <c r="I18">
+      <c r="I19">
         <v>71</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J19" s="6">
         <v>110</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="K19">
+        <v>110</v>
+      </c>
+      <c r="L19">
+        <v>179</v>
+      </c>
+      <c r="M19">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B20" s="16">
         <f>B14/B13</f>
         <v>0</v>
       </c>
-      <c r="C19" s="16">
-        <f t="shared" ref="C19:G19" si="0">C14/C13</f>
+      <c r="C20" s="16">
+        <f t="shared" ref="C20:G20" si="0">C14/C13</f>
         <v>0.50505050505050508</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D20" s="16">
         <f t="shared" si="0"/>
         <v>0.54040404040404044</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E20" s="16">
         <f t="shared" si="0"/>
         <v>0.54040404040404044</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F20" s="16">
         <f t="shared" si="0"/>
         <v>0.5505050505050505</v>
       </c>
-      <c r="G19" s="16">
+      <c r="G20" s="16">
         <f t="shared" si="0"/>
         <v>0.51712328767123283</v>
       </c>
-      <c r="H19" s="16">
-        <f t="shared" ref="H19:I19" si="1">H14/H13</f>
+      <c r="H20" s="16">
+        <f t="shared" ref="H20:I20" si="1">H14/H13</f>
         <v>0</v>
       </c>
-      <c r="I19" s="16">
+      <c r="I20" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J19" s="16">
-        <f t="shared" ref="J19" si="2">J14/J13</f>
+      <c r="J20" s="16">
+        <f t="shared" ref="J20:K20" si="2">J14/J13</f>
         <v>0.50929368029739774</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="K20" s="16">
+        <f t="shared" si="2"/>
+        <v>0.5938697318007663</v>
+      </c>
+      <c r="L20" s="16">
+        <f t="shared" ref="L20:M20" si="3">L14/L13</f>
+        <v>0.5938697318007663</v>
+      </c>
+      <c r="M20" s="16">
+        <f t="shared" si="3"/>
+        <v>0.5938697318007663</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="16">
-        <f>B18/B13</f>
+      <c r="B21" s="16">
+        <f>B19/B13</f>
         <v>0</v>
       </c>
-      <c r="C20" s="16">
-        <f t="shared" ref="C20:G20" si="3">C18/C13</f>
+      <c r="C21" s="16">
+        <f t="shared" ref="C21:G21" si="4">C19/C13</f>
         <v>0</v>
       </c>
-      <c r="D20" s="16">
-        <f t="shared" si="3"/>
+      <c r="D21" s="16">
+        <f t="shared" si="4"/>
         <v>0.45959595959595961</v>
       </c>
-      <c r="E20" s="16">
-        <f t="shared" si="3"/>
+      <c r="E21" s="16">
+        <f t="shared" si="4"/>
         <v>0.19191919191919191</v>
       </c>
-      <c r="F20" s="16">
-        <f t="shared" si="3"/>
+      <c r="F21" s="16">
+        <f t="shared" si="4"/>
         <v>0.20707070707070707</v>
       </c>
-      <c r="G20" s="16">
-        <f t="shared" si="3"/>
+      <c r="G21" s="16">
+        <f t="shared" si="4"/>
         <v>0.19178082191780821</v>
       </c>
-      <c r="H20" s="16">
-        <f t="shared" ref="H20:I20" si="4">H18/H13</f>
+      <c r="H21" s="16">
+        <f t="shared" ref="H21:I21" si="5">H19/H13</f>
         <v>0.22826086956521738</v>
       </c>
-      <c r="I20" s="16">
-        <f t="shared" si="4"/>
+      <c r="I21" s="16">
+        <f t="shared" si="5"/>
         <v>0.19293478260869565</v>
       </c>
-      <c r="J20" s="16">
-        <f t="shared" ref="J20" si="5">J18/J13</f>
+      <c r="J21" s="16">
+        <f t="shared" ref="J21:K21" si="6">J19/J13</f>
         <v>0.20446096654275092</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="K21" s="16">
+        <f t="shared" si="6"/>
+        <v>0.21072796934865901</v>
+      </c>
+      <c r="L21" s="16">
+        <f t="shared" ref="L21:M21" si="7">L19/L13</f>
+        <v>0.34291187739463602</v>
+      </c>
+      <c r="M21" s="16">
+        <f t="shared" si="7"/>
+        <v>0.17432950191570881</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="16">
-        <f>IF(B16=0,0,B17/B16)</f>
+      <c r="B22" s="16">
+        <f>IF(B17=0,0,B18/B17)</f>
         <v>0</v>
       </c>
-      <c r="C21" s="16">
-        <f t="shared" ref="C21:J21" si="6">IF(C16=0,0,C17/C16)</f>
+      <c r="C22" s="16">
+        <f t="shared" ref="C22:J22" si="8">IF(C17=0,0,C18/C17)</f>
         <v>0.20036429872495445</v>
       </c>
-      <c r="D21" s="16">
-        <f t="shared" si="6"/>
+      <c r="D22" s="16">
+        <f t="shared" si="8"/>
         <v>0.26463700234192039</v>
       </c>
-      <c r="E21" s="16">
-        <f t="shared" si="6"/>
+      <c r="E22" s="16">
+        <f t="shared" si="8"/>
         <v>0.16861826697892271</v>
       </c>
-      <c r="F21" s="16">
-        <f t="shared" si="6"/>
+      <c r="F22" s="16">
+        <f t="shared" si="8"/>
         <v>0.20300751879699247</v>
       </c>
-      <c r="G21" s="16">
-        <f t="shared" si="6"/>
+      <c r="G22" s="16">
+        <f t="shared" si="8"/>
         <v>0.17311233885819521</v>
       </c>
-      <c r="H21" s="16">
-        <f t="shared" si="6"/>
+      <c r="H22" s="16">
+        <f t="shared" si="8"/>
         <v>0.24722662440570523</v>
       </c>
-      <c r="I21" s="16">
-        <f t="shared" si="6"/>
+      <c r="I22" s="16">
+        <f t="shared" si="8"/>
         <v>0.18541996830427893</v>
       </c>
-      <c r="J21" s="16">
-        <f t="shared" si="6"/>
+      <c r="J22" s="16">
+        <f t="shared" si="8"/>
         <v>0.2139352306182532</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="K22" s="16">
+        <f t="shared" ref="K22:L22" si="9">IF(K17=0,0,K18/K17)</f>
+        <v>0.22022022022022023</v>
+      </c>
+      <c r="L22" s="16">
+        <f t="shared" si="9"/>
+        <v>0.46488549618320613</v>
+      </c>
+      <c r="M22" s="16">
+        <f t="shared" ref="M22" si="10">IF(M17=0,0,M18/M17)</f>
+        <v>0.17557251908396945</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23">
-        <v>-15</v>
-      </c>
-      <c r="D23">
-        <v>-15</v>
-      </c>
-      <c r="E23" s="5">
-        <v>-8</v>
-      </c>
-      <c r="F23">
-        <v>-8</v>
-      </c>
-      <c r="G23">
-        <v>-8</v>
-      </c>
-      <c r="H23">
-        <v>-8</v>
-      </c>
-      <c r="I23" s="5">
-        <v>-4</v>
-      </c>
-      <c r="J23">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>30</v>
       </c>
       <c r="C24">
-        <v>10</v>
+        <v>-15</v>
       </c>
       <c r="D24">
-        <v>10</v>
+        <v>-15</v>
       </c>
       <c r="E24" s="5">
-        <v>6</v>
+        <v>-8</v>
       </c>
       <c r="F24">
-        <v>6</v>
+        <v>-8</v>
       </c>
       <c r="G24">
-        <v>6</v>
+        <v>-8</v>
       </c>
       <c r="H24">
-        <v>6</v>
+        <v>-8</v>
       </c>
       <c r="I24" s="5">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="J24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+        <v>-4</v>
+      </c>
+      <c r="K24">
+        <v>-4</v>
+      </c>
+      <c r="L24">
+        <v>-4</v>
+      </c>
+      <c r="M24">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="13">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="C25">
         <v>10</v>
@@ -1232,205 +1406,305 @@
       <c r="D25">
         <v>10</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="5">
+        <v>6</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+      <c r="G25">
+        <v>6</v>
+      </c>
+      <c r="H25">
+        <v>6</v>
+      </c>
+      <c r="I25" s="5">
+        <v>4</v>
+      </c>
+      <c r="J25">
+        <v>4</v>
+      </c>
+      <c r="K25">
+        <v>4</v>
+      </c>
+      <c r="L25">
+        <v>4</v>
+      </c>
+      <c r="M25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="13">
         <v>10</v>
       </c>
-      <c r="F25">
+      <c r="C26">
         <v>10</v>
       </c>
-      <c r="G25">
+      <c r="D26">
         <v>10</v>
       </c>
-      <c r="H25">
+      <c r="E26">
         <v>10</v>
       </c>
-      <c r="I25">
+      <c r="F26">
         <v>10</v>
       </c>
-      <c r="J25">
+      <c r="G26">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="H26">
+        <v>10</v>
+      </c>
+      <c r="I26">
+        <v>10</v>
+      </c>
+      <c r="J26">
+        <v>10</v>
+      </c>
+      <c r="K26">
+        <v>10</v>
+      </c>
+      <c r="L26">
+        <v>10</v>
+      </c>
+      <c r="M26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B27" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <v>0.01</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D27" s="5">
         <v>0.02</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <v>0.02</v>
       </c>
-      <c r="F26">
+      <c r="F27">
         <v>0.02</v>
       </c>
-      <c r="G26">
+      <c r="G27">
         <v>0.02</v>
       </c>
-      <c r="H26">
+      <c r="H27">
         <v>0.02</v>
       </c>
-      <c r="I26">
+      <c r="I27">
         <v>0.02</v>
       </c>
-      <c r="J26">
+      <c r="J27">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="K27">
+        <v>0.02</v>
+      </c>
+      <c r="L27">
+        <v>0.02</v>
+      </c>
+      <c r="M27">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27">
+      <c r="B28" s="13"/>
+      <c r="C28">
         <v>1.3</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <v>1.3</v>
       </c>
-      <c r="E27">
+      <c r="E28">
         <v>1.3</v>
       </c>
-      <c r="F27">
+      <c r="F28">
         <v>1.3</v>
       </c>
-      <c r="G27">
+      <c r="G28">
         <v>1.3</v>
       </c>
-      <c r="H27">
+      <c r="H28">
         <v>1.3</v>
       </c>
-      <c r="I27">
+      <c r="I28">
         <v>1.3</v>
       </c>
-      <c r="J27">
+      <c r="J28">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="K28">
+        <v>1.3</v>
+      </c>
+      <c r="L28">
+        <v>1.3</v>
+      </c>
+      <c r="M28">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B29" s="9">
         <v>0.4</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>0.8</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <v>0.8</v>
       </c>
-      <c r="E28">
+      <c r="E29">
         <v>0.8</v>
       </c>
-      <c r="F28">
+      <c r="F29">
         <v>0.8</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <v>0.8</v>
       </c>
-      <c r="H28">
+      <c r="H29">
         <v>0.8</v>
       </c>
-      <c r="I28">
+      <c r="I29">
         <v>0.8</v>
       </c>
-      <c r="J28">
+      <c r="J29">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="8" t="s">
+      <c r="K29">
+        <v>0.8</v>
+      </c>
+      <c r="L29">
+        <v>0.8</v>
+      </c>
+      <c r="M29">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C30" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E30" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F30" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G30" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="H30" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I29" s="8" t="s">
+      <c r="I30" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J29" s="8" t="s">
+      <c r="J30" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="K30" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L30" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M30" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B31" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C31" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>23</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>23</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F31" t="s">
         <v>23</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G31" t="s">
         <v>23</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H31" t="s">
         <v>23</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I31" t="s">
         <v>23</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J31" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="K31" t="s">
+        <v>23</v>
+      </c>
+      <c r="L31" t="s">
+        <v>23</v>
+      </c>
+      <c r="M31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7" t="s">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E33" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F33" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="G33" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L33" s="7" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>